<commit_message>
fix: Clean up thread size encoding issues
Fixed 376 products with garbled thread size characters.

Before: "1/4 â€" 19" (UTF-8 encoding corruption)
After: "1/4 - 19" (clean ASCII dash)

This fixes the display issue in Excel where thread sizes showed
"â€"" instead of proper dash characters.
</commit_message>
<xml_diff>
--- a/data/balflex_heizmann_PRESSARMATUREN_WITH_SERIES.xlsx
+++ b/data/balflex_heizmann_PRESSARMATUREN_WITH_SERIES.xlsx
@@ -54668,7 +54668,7 @@
       </c>
       <c r="Y426" t="inlineStr">
         <is>
-          <t>1.1/4 â€“ 11</t>
+          <t>1.1/4 - 11</t>
         </is>
       </c>
       <c r="Z426" t="n">
@@ -54790,7 +54790,7 @@
       </c>
       <c r="Y427" t="inlineStr">
         <is>
-          <t>1/4 â€“ 19</t>
+          <t>1/4 - 19</t>
         </is>
       </c>
       <c r="Z427" t="n">
@@ -54912,7 +54912,7 @@
       </c>
       <c r="Y428" t="inlineStr">
         <is>
-          <t>3/8 â€“ 19</t>
+          <t>3/8 - 19</t>
         </is>
       </c>
       <c r="Z428" t="n">
@@ -55490,7 +55490,7 @@
       </c>
       <c r="Y433" t="inlineStr">
         <is>
-          <t>1/4 â€“ 19</t>
+          <t>1/4 - 19</t>
         </is>
       </c>
       <c r="Z433" t="n">
@@ -55612,7 +55612,7 @@
       </c>
       <c r="Y434" t="inlineStr">
         <is>
-          <t>3/8 â€“ 19</t>
+          <t>3/8 - 19</t>
         </is>
       </c>
       <c r="Z434" t="n">
@@ -57110,7 +57110,7 @@
       </c>
       <c r="Y447" t="inlineStr">
         <is>
-          <t>3/8 â€“ 19</t>
+          <t>3/8 - 19</t>
         </is>
       </c>
       <c r="Z447" t="n">
@@ -57798,7 +57798,7 @@
       </c>
       <c r="Y453" t="inlineStr">
         <is>
-          <t>1.1/4 â€“ 11</t>
+          <t>1.1/4 - 11</t>
         </is>
       </c>
       <c r="Z453" t="n">

</xml_diff>